<commit_message>
complete fix error import group and addtion back to top
</commit_message>
<xml_diff>
--- a/import/List_group_DH.xlsx
+++ b/import/List_group_DH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\L A P T R I N H V I EN WEBSITE\Cd2\nckh_ng\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E16E85-FC95-4E43-B568-2500FD29953D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780033F5-93AE-4011-A7BE-CB11D11AC5E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E6A71C13-185B-42A7-A4FA-5B290892829C}"/>
   </bookViews>
@@ -38,12 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="61">
   <si>
-    <t>23211TT2984</t>
-  </si>
-  <si>
-    <t>23211TT1404</t>
-  </si>
-  <si>
     <t>NT</t>
   </si>
   <si>
@@ -65,90 +59,6 @@
     <t>SINH_VIEN</t>
   </si>
   <si>
-    <t>23211TT3144</t>
-  </si>
-  <si>
-    <t>21211TT3802</t>
-  </si>
-  <si>
-    <t>21211TT4493</t>
-  </si>
-  <si>
-    <t>21211TT4824</t>
-  </si>
-  <si>
-    <t>22211TT2183</t>
-  </si>
-  <si>
-    <t>22211TT3455</t>
-  </si>
-  <si>
-    <t>23211TT0403</t>
-  </si>
-  <si>
-    <t>23211TT0774</t>
-  </si>
-  <si>
-    <t>22211TT2666</t>
-  </si>
-  <si>
-    <t>23211TT4312</t>
-  </si>
-  <si>
-    <t>23211TT3424</t>
-  </si>
-  <si>
-    <t>23211TT1158</t>
-  </si>
-  <si>
-    <t>23211TT0068</t>
-  </si>
-  <si>
-    <t>23211TT0659</t>
-  </si>
-  <si>
-    <t>22211TT3957</t>
-  </si>
-  <si>
-    <t>23211TT0087</t>
-  </si>
-  <si>
-    <t>23211TT2438</t>
-  </si>
-  <si>
-    <t>21211TT1402</t>
-  </si>
-  <si>
-    <t>23211TT4636</t>
-  </si>
-  <si>
-    <t>23211TT4524</t>
-  </si>
-  <si>
-    <t>23211TT4445</t>
-  </si>
-  <si>
-    <t>22211TT3477</t>
-  </si>
-  <si>
-    <t>23211TT0653</t>
-  </si>
-  <si>
-    <t>23211TT0388</t>
-  </si>
-  <si>
-    <t>23211TT4339</t>
-  </si>
-  <si>
-    <t>23211TT4749</t>
-  </si>
-  <si>
-    <t>23211TT0610</t>
-  </si>
-  <si>
-    <t>23211TT3247</t>
-  </si>
-  <si>
     <t>23211TT1174</t>
   </si>
   <si>
@@ -158,27 +68,6 @@
     <t>23211TT0117</t>
   </si>
   <si>
-    <t>22211TT3094</t>
-  </si>
-  <si>
-    <t>23211TT2327</t>
-  </si>
-  <si>
-    <t>23211TT2360</t>
-  </si>
-  <si>
-    <t>23211TT0564</t>
-  </si>
-  <si>
-    <t>22211TT3655</t>
-  </si>
-  <si>
-    <t>22211TT4827</t>
-  </si>
-  <si>
-    <t>23211TT4803</t>
-  </si>
-  <si>
     <t>NHOM_1</t>
   </si>
   <si>
@@ -206,19 +95,130 @@
     <t>NHOM_9</t>
   </si>
   <si>
-    <t>21211TT3805</t>
-  </si>
-  <si>
-    <t>22211TT0255</t>
-  </si>
-  <si>
-    <t>22211TT2665</t>
-  </si>
-  <si>
     <t>23211TT1234</t>
   </si>
   <si>
     <t>22211TT1234</t>
+  </si>
+  <si>
+    <t>23211DH0001</t>
+  </si>
+  <si>
+    <t>23211DH0002</t>
+  </si>
+  <si>
+    <t>23211DH0003</t>
+  </si>
+  <si>
+    <t>23211DH0004</t>
+  </si>
+  <si>
+    <t>23211DH0005</t>
+  </si>
+  <si>
+    <t>23211DH0006</t>
+  </si>
+  <si>
+    <t>23211DH0007</t>
+  </si>
+  <si>
+    <t>23211DH0008</t>
+  </si>
+  <si>
+    <t>23211DH0009</t>
+  </si>
+  <si>
+    <t>23211DH0010</t>
+  </si>
+  <si>
+    <t>23211DH0011</t>
+  </si>
+  <si>
+    <t>23211DH0012</t>
+  </si>
+  <si>
+    <t>23211DH0013</t>
+  </si>
+  <si>
+    <t>23211DH0014</t>
+  </si>
+  <si>
+    <t>23211DH0015</t>
+  </si>
+  <si>
+    <t>23211DH0016</t>
+  </si>
+  <si>
+    <t>23211DH0017</t>
+  </si>
+  <si>
+    <t>23211DH0018</t>
+  </si>
+  <si>
+    <t>23211DH0019</t>
+  </si>
+  <si>
+    <t>23211DH0020</t>
+  </si>
+  <si>
+    <t>23211DH0021</t>
+  </si>
+  <si>
+    <t>23211DH0022</t>
+  </si>
+  <si>
+    <t>23211DH0023</t>
+  </si>
+  <si>
+    <t>23211DH0024</t>
+  </si>
+  <si>
+    <t>23211DH0025</t>
+  </si>
+  <si>
+    <t>23211DH0026</t>
+  </si>
+  <si>
+    <t>23211DH0027</t>
+  </si>
+  <si>
+    <t>23211DH0028</t>
+  </si>
+  <si>
+    <t>23211DH0029</t>
+  </si>
+  <si>
+    <t>23211DH0030</t>
+  </si>
+  <si>
+    <t>23211DH0031</t>
+  </si>
+  <si>
+    <t>23211DH0032</t>
+  </si>
+  <si>
+    <t>23211DH0033</t>
+  </si>
+  <si>
+    <t>23211DH0034</t>
+  </si>
+  <si>
+    <t>23211DH0035</t>
+  </si>
+  <si>
+    <t>23211DH0036</t>
+  </si>
+  <si>
+    <t>23211DH0037</t>
+  </si>
+  <si>
+    <t>23211DH0038</t>
+  </si>
+  <si>
+    <t>23211DH0039</t>
+  </si>
+  <si>
+    <t>23211DH0040</t>
   </si>
 </sst>
 </file>
@@ -752,7 +752,7 @@
   <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
@@ -766,542 +766,542 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2" s="6">
         <v>1</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" s="6">
         <v>1</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4" s="6">
         <v>1</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" s="6">
         <v>1</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6" s="6">
         <v>1</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7" s="8">
         <v>2</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C8" s="8">
         <v>2</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C9" s="8">
         <v>2</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C10" s="8">
         <v>2</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C11" s="8">
         <v>2</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C12" s="10">
         <v>3</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13" s="10">
         <v>3</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C14" s="10">
         <v>3</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C15" s="10">
         <v>3</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C16" s="10">
         <v>3</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C17" s="12">
         <v>4</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C18" s="12">
         <v>4</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C19" s="12">
         <v>4</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C20" s="12">
         <v>4</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C21" s="12">
         <v>4</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C22" s="14">
         <v>5</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C23" s="14">
         <v>5</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C24" s="14">
         <v>5</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="13" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C25" s="14">
         <v>5</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C26" s="14">
         <v>5</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="15" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C27" s="16">
         <v>6</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="15" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C28" s="16">
         <v>6</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="15" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C29" s="16">
         <v>6</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="15" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C30" s="16">
         <v>6</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="15" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C31" s="16">
         <v>6</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="17" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C32" s="18">
         <v>7</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="17" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C33" s="18">
         <v>7</v>
       </c>
       <c r="D33" s="22" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="17" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C34" s="18">
         <v>7</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="17" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C35" s="18">
         <v>7</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="17" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C36" s="18">
         <v>7</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="19" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C37" s="20">
         <v>8</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="19" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C38" s="20">
         <v>8</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="19" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C39" s="20">
         <v>8</v>
@@ -1312,100 +1312,100 @@
     </row>
     <row r="40" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="19" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C40" s="20">
         <v>8</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="19" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C41" s="20">
         <v>8</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C42" s="4">
         <v>9</v>
       </c>
       <c r="D42" s="21" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C43" s="4">
         <v>9</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C44" s="4">
         <v>9</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C45" s="4">
         <v>9</v>
       </c>
       <c r="D45" s="22" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C46" s="4">
         <v>9</v>
       </c>
       <c r="D46" s="21" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>